<commit_message>
0.0.9: fix bug on empty array support.
</commit_message>
<xml_diff>
--- a/meta/objects/CodeDefinition2.xlsx
+++ b/meta/objects/CodeDefinition2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC756D67-618D-0840-A035-986045CEDA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958D5104-7F1E-0A48-87C1-660E76FABBD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1860" windowWidth="29040" windowHeight="15840" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
   <si>
     <t>クラス名</t>
   </si>
@@ -521,6 +521,10 @@
   </si>
   <si>
     <t>listOf&lt;String&gt;()</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>numList</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1218,7 +1222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1352,9 +1356,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1890,7 +1891,7 @@
   <dimension ref="A1:W59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1947,7 +1948,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="90"/>
+      <c r="K5" s="89"/>
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
@@ -1968,7 +1969,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
-      <c r="K6" s="89"/>
+      <c r="K6" s="88"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
@@ -1990,7 +1991,7 @@
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
       <c r="J7" s="30"/>
-      <c r="K7" s="89"/>
+      <c r="K7" s="88"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
       <c r="Q7" s="30"/>
@@ -2010,7 +2011,7 @@
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
       <c r="J8" s="30"/>
-      <c r="K8" s="89" t="s">
+      <c r="K8" s="88" t="s">
         <v>50</v>
       </c>
       <c r="O8" s="30"/>
@@ -2020,10 +2021,10 @@
       <c r="S8" s="31"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="119" t="s">
+      <c r="A9" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="120"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="10" t="s">
         <v>54</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>50</v>
       </c>
       <c r="J9" s="30"/>
-      <c r="K9" s="89"/>
+      <c r="K9" s="88"/>
       <c r="O9" s="30" t="s">
         <v>50</v>
       </c>
@@ -2060,7 +2061,7 @@
       <c r="H10" s="30"/>
       <c r="I10" s="30"/>
       <c r="J10" s="30"/>
-      <c r="K10" s="89"/>
+      <c r="K10" s="88"/>
       <c r="O10" s="30"/>
       <c r="P10" s="30"/>
       <c r="Q10" s="30"/>
@@ -2068,40 +2069,40 @@
       <c r="S10" s="31"/>
     </row>
     <row r="11" spans="1:21" s="25" customFormat="1">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="86" t="s">
+      <c r="B11" s="84"/>
+      <c r="C11" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="89"/>
-      <c r="I11" s="89"/>
-      <c r="K11" s="89"/>
-      <c r="O11" s="89"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="O11" s="88"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="122"/>
-      <c r="E12" s="122"/>
-      <c r="F12" s="123"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="122"/>
       <c r="G12" s="61"/>
       <c r="H12" s="61"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="91"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="92"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91"/>
       <c r="O12" s="61"/>
       <c r="P12" s="61"/>
       <c r="Q12" s="61"/>
@@ -2125,7 +2126,7 @@
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
-      <c r="K13" s="89"/>
+      <c r="K13" s="88"/>
       <c r="O13" s="30"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
@@ -2210,10 +2211,10 @@
       <c r="S16"/>
     </row>
     <row r="17" spans="1:23" s="25" customFormat="1">
-      <c r="A17" s="124" t="s">
+      <c r="A17" s="123" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="125"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="60"/>
       <c r="D17" t="s">
         <v>52</v>
@@ -2306,10 +2307,10 @@
       <c r="S20"/>
     </row>
     <row r="21" spans="1:23" s="25" customFormat="1">
-      <c r="A21" s="124" t="s">
+      <c r="A21" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="125"/>
+      <c r="B21" s="124"/>
       <c r="C21" s="60" t="s">
         <v>31</v>
       </c>
@@ -2391,10 +2392,10 @@
       <c r="H24" s="63"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
-      <c r="K24" s="93"/>
-      <c r="L24" s="93"/>
-      <c r="M24" s="93"/>
-      <c r="N24" s="93"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="92"/>
+      <c r="M24" s="92"/>
+      <c r="N24" s="92"/>
       <c r="O24" s="63"/>
       <c r="P24" s="63"/>
       <c r="Q24" s="63"/>
@@ -2498,10 +2499,10 @@
       <c r="H29" s="63"/>
       <c r="I29" s="63"/>
       <c r="J29" s="63"/>
-      <c r="K29" s="93"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="93"/>
-      <c r="N29" s="93"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="92"/>
+      <c r="M29" s="92"/>
+      <c r="N29" s="92"/>
       <c r="O29" s="63"/>
       <c r="P29" s="63"/>
       <c r="Q29" s="63"/>
@@ -2523,10 +2524,10 @@
       <c r="H30" s="64"/>
       <c r="I30" s="64"/>
       <c r="J30" s="64"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
-      <c r="M30" s="94"/>
-      <c r="N30" s="94"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="93"/>
+      <c r="M30" s="93"/>
+      <c r="N30" s="93"/>
       <c r="O30" s="64"/>
       <c r="P30" s="64"/>
       <c r="Q30" s="64"/>
@@ -2548,10 +2549,10 @@
       <c r="H31" s="64"/>
       <c r="I31" s="64"/>
       <c r="J31" s="64"/>
-      <c r="K31" s="94"/>
-      <c r="L31" s="94"/>
-      <c r="M31" s="94"/>
-      <c r="N31" s="94"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="93"/>
+      <c r="N31" s="93"/>
       <c r="O31" s="64"/>
       <c r="P31" s="64"/>
       <c r="Q31" s="64"/>
@@ -2573,10 +2574,10 @@
       <c r="H32" s="64"/>
       <c r="I32" s="64"/>
       <c r="J32" s="64"/>
-      <c r="K32" s="94"/>
-      <c r="L32" s="94"/>
-      <c r="M32" s="94"/>
-      <c r="N32" s="94"/>
+      <c r="K32" s="93"/>
+      <c r="L32" s="93"/>
+      <c r="M32" s="93"/>
+      <c r="N32" s="93"/>
       <c r="O32" s="64"/>
       <c r="P32" s="64"/>
       <c r="Q32" s="64"/>
@@ -2648,10 +2649,10 @@
       <c r="H35" s="63"/>
       <c r="I35" s="63"/>
       <c r="J35" s="63"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="93"/>
-      <c r="N35" s="93"/>
+      <c r="K35" s="92"/>
+      <c r="L35" s="92"/>
+      <c r="M35" s="92"/>
+      <c r="N35" s="92"/>
       <c r="O35" s="63"/>
       <c r="P35" s="63"/>
       <c r="Q35" s="63"/>
@@ -2677,10 +2678,10 @@
       <c r="H36" s="64"/>
       <c r="I36" s="64"/>
       <c r="J36" s="64"/>
-      <c r="K36" s="94"/>
-      <c r="L36" s="94"/>
-      <c r="M36" s="94"/>
-      <c r="N36" s="94"/>
+      <c r="K36" s="93"/>
+      <c r="L36" s="93"/>
+      <c r="M36" s="93"/>
+      <c r="N36" s="93"/>
       <c r="O36" s="64"/>
       <c r="P36" s="64"/>
       <c r="Q36" s="64"/>
@@ -2706,10 +2707,10 @@
       <c r="H37" s="64"/>
       <c r="I37" s="64"/>
       <c r="J37" s="64"/>
-      <c r="K37" s="94"/>
-      <c r="L37" s="94"/>
-      <c r="M37" s="94"/>
-      <c r="N37" s="94"/>
+      <c r="K37" s="93"/>
+      <c r="L37" s="93"/>
+      <c r="M37" s="93"/>
+      <c r="N37" s="93"/>
       <c r="O37" s="64"/>
       <c r="P37" s="64"/>
       <c r="Q37" s="64"/>
@@ -2731,10 +2732,10 @@
       <c r="H38" s="64"/>
       <c r="I38" s="64"/>
       <c r="J38" s="64"/>
-      <c r="K38" s="94"/>
-      <c r="L38" s="94"/>
-      <c r="M38" s="94"/>
-      <c r="N38" s="94"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="93"/>
+      <c r="M38" s="93"/>
+      <c r="N38" s="93"/>
       <c r="O38" s="64"/>
       <c r="P38" s="64"/>
       <c r="Q38" s="64"/>
@@ -2805,10 +2806,10 @@
       <c r="H41" s="63"/>
       <c r="I41" s="63"/>
       <c r="J41" s="63"/>
-      <c r="K41" s="93"/>
-      <c r="L41" s="93"/>
-      <c r="M41" s="93"/>
-      <c r="N41" s="93"/>
+      <c r="K41" s="92"/>
+      <c r="L41" s="92"/>
+      <c r="M41" s="92"/>
+      <c r="N41" s="92"/>
       <c r="O41" s="63"/>
       <c r="P41" s="63"/>
       <c r="Q41" s="63"/>
@@ -2830,10 +2831,10 @@
       <c r="H42" s="64"/>
       <c r="I42" s="64"/>
       <c r="J42" s="64"/>
-      <c r="K42" s="94"/>
-      <c r="L42" s="94"/>
-      <c r="M42" s="94"/>
-      <c r="N42" s="94"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="93"/>
       <c r="O42" s="64"/>
       <c r="P42" s="64"/>
       <c r="Q42" s="64"/>
@@ -2855,10 +2856,10 @@
       <c r="H43" s="64"/>
       <c r="I43" s="64"/>
       <c r="J43" s="64"/>
-      <c r="K43" s="94"/>
-      <c r="L43" s="94"/>
-      <c r="M43" s="94"/>
-      <c r="N43" s="94"/>
+      <c r="K43" s="93"/>
+      <c r="L43" s="93"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="93"/>
       <c r="O43" s="64"/>
       <c r="P43" s="64"/>
       <c r="Q43" s="64"/>
@@ -2880,10 +2881,10 @@
       <c r="H44" s="64"/>
       <c r="I44" s="64"/>
       <c r="J44" s="64"/>
-      <c r="K44" s="94"/>
-      <c r="L44" s="94"/>
-      <c r="M44" s="94"/>
-      <c r="N44" s="94"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
       <c r="O44" s="64"/>
       <c r="P44" s="64"/>
       <c r="Q44" s="64"/>
@@ -2944,89 +2945,89 @@
       <c r="W46" s="15"/>
     </row>
     <row r="47" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A47" s="127" t="s">
+      <c r="A47" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="127" t="s">
+      <c r="B47" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="126" t="s">
+      <c r="C47" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="126" t="s">
+      <c r="D47" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="113" t="s">
+      <c r="E47" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="126" t="s">
+      <c r="F47" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="113" t="s">
+      <c r="G47" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="H47" s="113" t="s">
+      <c r="H47" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="I47" s="115" t="s">
+      <c r="I47" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="J47" s="117" t="s">
+      <c r="J47" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="K47" s="112" t="s">
+      <c r="K47" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="L47" s="112" t="s">
+      <c r="L47" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="M47" s="112" t="s">
+      <c r="M47" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="N47" s="112" t="s">
+      <c r="N47" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="O47" s="129" t="s">
+      <c r="O47" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="P47" s="115" t="s">
+      <c r="P47" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="Q47" s="115" t="s">
+      <c r="Q47" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="R47" s="117" t="s">
+      <c r="R47" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="S47" s="126" t="s">
+      <c r="S47" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="T47" s="126"/>
+      <c r="T47" s="125"/>
       <c r="U47" s="16"/>
       <c r="V47" s="17"/>
       <c r="W47" s="9"/>
     </row>
     <row r="48" spans="1:23">
-      <c r="A48" s="127"/>
-      <c r="B48" s="127"/>
-      <c r="C48" s="126"/>
-      <c r="D48" s="126"/>
-      <c r="E48" s="128"/>
-      <c r="F48" s="126"/>
-      <c r="G48" s="114"/>
-      <c r="H48" s="114"/>
-      <c r="I48" s="116"/>
-      <c r="J48" s="118"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="112"/>
-      <c r="M48" s="112"/>
-      <c r="N48" s="112"/>
-      <c r="O48" s="130"/>
-      <c r="P48" s="116"/>
-      <c r="Q48" s="116"/>
-      <c r="R48" s="118"/>
-      <c r="S48" s="126"/>
-      <c r="T48" s="126"/>
+      <c r="A48" s="126"/>
+      <c r="B48" s="126"/>
+      <c r="C48" s="125"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="127"/>
+      <c r="F48" s="125"/>
+      <c r="G48" s="113"/>
+      <c r="H48" s="113"/>
+      <c r="I48" s="115"/>
+      <c r="J48" s="117"/>
+      <c r="K48" s="111"/>
+      <c r="L48" s="111"/>
+      <c r="M48" s="111"/>
+      <c r="N48" s="111"/>
+      <c r="O48" s="129"/>
+      <c r="P48" s="115"/>
+      <c r="Q48" s="115"/>
+      <c r="R48" s="117"/>
+      <c r="S48" s="125"/>
+      <c r="T48" s="125"/>
       <c r="U48" s="18"/>
       <c r="V48" s="22"/>
       <c r="W48" s="15"/>
@@ -3048,15 +3049,15 @@
       </c>
       <c r="G49" s="19"/>
       <c r="H49" s="70"/>
-      <c r="I49" s="103"/>
-      <c r="J49" s="103"/>
-      <c r="K49" s="95"/>
-      <c r="L49" s="95"/>
-      <c r="M49" s="95"/>
-      <c r="N49" s="104"/>
-      <c r="O49" s="103"/>
-      <c r="P49" s="103"/>
-      <c r="Q49" s="105"/>
+      <c r="I49" s="102"/>
+      <c r="J49" s="102"/>
+      <c r="K49" s="94"/>
+      <c r="L49" s="94"/>
+      <c r="M49" s="94"/>
+      <c r="N49" s="103"/>
+      <c r="O49" s="102"/>
+      <c r="P49" s="102"/>
+      <c r="Q49" s="104"/>
       <c r="R49" s="70" t="s">
         <v>31</v>
       </c>
@@ -3069,17 +3070,17 @@
       <c r="W49" s="15"/>
     </row>
     <row r="50" spans="1:23">
-      <c r="A50" s="81">
+      <c r="A50" s="80">
         <f>A49+1</f>
         <v>2</v>
       </c>
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="81" t="s">
         <v>55</v>
       </c>
       <c r="C50" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="82"/>
+      <c r="D50" s="81"/>
       <c r="E50" s="19"/>
       <c r="F50" s="19" t="s">
         <v>57</v>
@@ -3088,13 +3089,13 @@
       <c r="H50" s="70"/>
       <c r="I50" s="70"/>
       <c r="J50" s="70"/>
-      <c r="K50" s="96"/>
-      <c r="L50" s="96"/>
-      <c r="M50" s="111"/>
-      <c r="N50" s="96"/>
+      <c r="K50" s="95"/>
+      <c r="L50" s="95"/>
+      <c r="M50" s="110"/>
+      <c r="N50" s="95"/>
       <c r="O50" s="70"/>
       <c r="P50" s="70"/>
-      <c r="Q50" s="106"/>
+      <c r="Q50" s="105"/>
       <c r="R50" s="70" t="s">
         <v>31</v>
       </c>
@@ -3103,21 +3104,21 @@
       </c>
       <c r="T50" s="20"/>
       <c r="U50" s="20"/>
-      <c r="V50" s="83"/>
+      <c r="V50" s="82"/>
       <c r="W50" s="15"/>
     </row>
     <row r="51" spans="1:23">
-      <c r="A51" s="81">
+      <c r="A51" s="80">
         <f t="shared" ref="A51:A52" si="0">A50+1</f>
         <v>3</v>
       </c>
-      <c r="B51" s="82" t="s">
+      <c r="B51" s="81" t="s">
         <v>82</v>
       </c>
       <c r="C51" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="82" t="s">
+      <c r="D51" s="81" t="s">
         <v>56</v>
       </c>
       <c r="E51" s="19"/>
@@ -3126,19 +3127,19 @@
       <c r="H51" s="70"/>
       <c r="I51" s="70"/>
       <c r="J51" s="70"/>
-      <c r="K51" s="96" t="s">
+      <c r="K51" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="L51" s="96" t="s">
+      <c r="L51" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="M51" s="111"/>
-      <c r="N51" s="96" t="s">
+      <c r="M51" s="110"/>
+      <c r="N51" s="95" t="s">
         <v>86</v>
       </c>
       <c r="O51" s="70"/>
       <c r="P51" s="70"/>
-      <c r="Q51" s="106"/>
+      <c r="Q51" s="105"/>
       <c r="R51" s="70" t="s">
         <v>31</v>
       </c>
@@ -3147,21 +3148,21 @@
       </c>
       <c r="T51" s="20"/>
       <c r="U51" s="20"/>
-      <c r="V51" s="83"/>
+      <c r="V51" s="82"/>
       <c r="W51" s="15"/>
     </row>
     <row r="52" spans="1:23">
-      <c r="A52" s="81">
+      <c r="A52" s="80">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B52" s="82" t="s">
+      <c r="B52" s="81" t="s">
         <v>83</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="82"/>
+      <c r="D52" s="81"/>
       <c r="E52" s="19"/>
       <c r="F52" s="19" t="s">
         <v>57</v>
@@ -3170,13 +3171,13 @@
       <c r="H52" s="70"/>
       <c r="I52" s="70"/>
       <c r="J52" s="70"/>
-      <c r="K52" s="96"/>
-      <c r="L52" s="96"/>
-      <c r="M52" s="111"/>
-      <c r="N52" s="96"/>
+      <c r="K52" s="95"/>
+      <c r="L52" s="95"/>
+      <c r="M52" s="110"/>
+      <c r="N52" s="95"/>
       <c r="O52" s="70"/>
       <c r="P52" s="70"/>
-      <c r="Q52" s="106"/>
+      <c r="Q52" s="105"/>
       <c r="R52" s="70" t="s">
         <v>31</v>
       </c>
@@ -3185,21 +3186,21 @@
       </c>
       <c r="T52" s="20"/>
       <c r="U52" s="20"/>
-      <c r="V52" s="83"/>
+      <c r="V52" s="82"/>
       <c r="W52" s="15"/>
     </row>
     <row r="53" spans="1:23">
-      <c r="A53" s="81">
-        <f t="shared" ref="A53" si="1">A52+1</f>
+      <c r="A53" s="80">
+        <f t="shared" ref="A53:A54" si="1">A52+1</f>
         <v>5</v>
       </c>
-      <c r="B53" s="82" t="s">
+      <c r="B53" s="81" t="s">
         <v>84</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="82"/>
+      <c r="D53" s="81"/>
       <c r="E53" s="19"/>
       <c r="F53" s="19" t="s">
         <v>57</v>
@@ -3208,13 +3209,13 @@
       <c r="H53" s="70"/>
       <c r="I53" s="70"/>
       <c r="J53" s="70"/>
-      <c r="K53" s="96"/>
-      <c r="L53" s="96"/>
-      <c r="M53" s="111"/>
-      <c r="N53" s="96"/>
+      <c r="K53" s="95"/>
+      <c r="L53" s="95"/>
+      <c r="M53" s="110"/>
+      <c r="N53" s="95"/>
       <c r="O53" s="70"/>
       <c r="P53" s="70"/>
-      <c r="Q53" s="106"/>
+      <c r="Q53" s="105"/>
       <c r="R53" s="70" t="s">
         <v>31</v>
       </c>
@@ -3223,32 +3224,43 @@
       </c>
       <c r="T53" s="20"/>
       <c r="U53" s="20"/>
-      <c r="V53" s="83"/>
+      <c r="V53" s="82"/>
       <c r="W53" s="15"/>
     </row>
     <row r="54" spans="1:23">
-      <c r="A54" s="75"/>
-      <c r="B54" s="76"/>
-      <c r="C54" s="77"/>
-      <c r="D54" s="76"/>
-      <c r="E54" s="77"/>
-      <c r="F54" s="77"/>
-      <c r="G54" s="77"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="107"/>
-      <c r="J54" s="78"/>
-      <c r="K54" s="108"/>
-      <c r="L54" s="109"/>
-      <c r="M54" s="108"/>
-      <c r="N54" s="109"/>
-      <c r="O54" s="107"/>
-      <c r="P54" s="107"/>
-      <c r="Q54" s="110"/>
-      <c r="R54" s="78"/>
-      <c r="S54" s="77"/>
-      <c r="T54" s="79"/>
-      <c r="U54" s="79"/>
-      <c r="V54" s="80"/>
+      <c r="A54" s="80">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B54" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="77"/>
+      <c r="I54" s="106"/>
+      <c r="J54" s="77"/>
+      <c r="K54" s="107"/>
+      <c r="L54" s="108"/>
+      <c r="M54" s="107"/>
+      <c r="N54" s="108"/>
+      <c r="O54" s="106"/>
+      <c r="P54" s="106"/>
+      <c r="Q54" s="109"/>
+      <c r="R54" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="S54" s="76"/>
+      <c r="T54" s="78"/>
+      <c r="U54" s="78"/>
+      <c r="V54" s="79"/>
       <c r="W54" s="15"/>
     </row>
     <row r="55" spans="1:23">
@@ -3258,24 +3270,24 @@
       <c r="N55" s="40"/>
     </row>
     <row r="56" spans="1:23">
-      <c r="K56" s="99"/>
-      <c r="L56" s="99"/>
-      <c r="M56" s="99"/>
+      <c r="K56" s="98"/>
+      <c r="L56" s="98"/>
+      <c r="M56" s="98"/>
       <c r="N56" s="40"/>
     </row>
     <row r="57" spans="1:23">
-      <c r="K57" s="99"/>
-      <c r="L57" s="99"/>
-      <c r="M57" s="99"/>
+      <c r="K57" s="98"/>
+      <c r="L57" s="98"/>
+      <c r="M57" s="98"/>
       <c r="N57" s="40"/>
     </row>
     <row r="58" spans="1:23">
-      <c r="M58" s="97"/>
+      <c r="M58" s="96"/>
     </row>
     <row r="59" spans="1:23">
-      <c r="K59" s="98"/>
-      <c r="L59" s="98"/>
-      <c r="M59" s="98"/>
+      <c r="K59" s="97"/>
+      <c r="L59" s="97"/>
+      <c r="M59" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -3443,7 +3455,7 @@
       <c r="L4" s="54"/>
       <c r="N4" s="54"/>
       <c r="P4" s="54"/>
-      <c r="R4" s="100"/>
+      <c r="R4" s="99"/>
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="55" t="s">
@@ -3466,13 +3478,13 @@
       <c r="P5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="101" t="s">
+      <c r="R5" s="100" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="57"/>
-      <c r="R6" s="102" t="s">
+      <c r="R6" s="101" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>